<commit_message>
Add GPS mop up
</commit_message>
<xml_diff>
--- a/app/designerFiles/app/config/tables/sample/forms/sample/sample.xlsx
+++ b/app/designerFiles/app/config/tables/sample/forms/sample/sample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14000" windowWidth="24640" xWindow="700" yWindow="900"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16440" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="choices" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1" refMode="R1C1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -405,20 +405,20 @@
   </sheetPr>
   <dimension ref="A1:AF124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0" zoomScale="75">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A17" workbookViewId="0" zoomScale="75">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col bestFit="1" customWidth="1" max="4" min="4" width="50.5"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" width="14.6640625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" width="13.83203125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" width="14.625"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" width="13.875"/>
     <col bestFit="1" customWidth="1" max="7" min="7" width="28"/>
     <col bestFit="1" customWidth="1" max="8" min="8" width="22"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="17" r="1">
+    <row r="1">
       <c r="A1" t="inlineStr"/>
       <c r="B1" t="inlineStr">
         <is>
@@ -651,7 +651,11 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>healthcare_worker_name</t>
+        </is>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>select_one</t>
@@ -825,7 +829,11 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>consent_paper</t>
+        </is>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>select_one</t>
@@ -952,7 +960,7 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" t="inlineStr"/>
     </row>
-    <row customFormat="1" customHeight="1" ht="17.75" r="12" s="6">
+    <row customFormat="1" customHeight="1" ht="17.85" r="12" s="6">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
@@ -1299,7 +1307,11 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>sample_type</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>select_multiple</t>
@@ -1735,7 +1747,11 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>temp_consent</t>
+        </is>
+      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t xml:space="preserve">select_one </t>
@@ -2837,7 +2853,11 @@
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>scan_another_2</t>
+        </is>
+      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>select_one</t>
@@ -3287,7 +3307,11 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>scan_another_3</t>
+        </is>
+      </c>
       <c r="F68" t="inlineStr">
         <is>
           <t>select_one</t>
@@ -3913,7 +3937,11 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
       <c r="D83" t="inlineStr"/>
-      <c r="E83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>scan_another_4</t>
+        </is>
+      </c>
       <c r="F83" t="inlineStr">
         <is>
           <t>select_one</t>
@@ -5765,7 +5793,7 @@
       <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -6192,13 +6220,13 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="30.83203125"/>
+    <col customWidth="1" max="1" min="1" width="30.875"/>
     <col customWidth="1" max="2" min="2" width="20"/>
   </cols>
   <sheetData>
@@ -6250,7 +6278,7 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -6261,7 +6289,7 @@
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>New Sample</t>
+          <t>New Biological Sample</t>
         </is>
       </c>
     </row>
@@ -6276,16 +6304,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:C1"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" width="20.83203125"/>
-    <col bestFit="1" customWidth="1" max="3" min="2" width="22.1640625"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" width="20.875"/>
+    <col bestFit="1" customWidth="1" max="3" min="2" width="22.125"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6784,6 +6812,142 @@
         </is>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>temp_consent</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C35" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>temp_consent</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>scan_another_2</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C38" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>scan_another_2</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>scan_another_3</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C41" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>scan_another_3</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C42" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>scan_another_4</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="C44" s="5" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>scan_another_4</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="C45" s="5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>